<commit_message>
PI 3 update 1
</commit_message>
<xml_diff>
--- a/Sprint_5/FO.BD.GDC.SDC.005-001.xlsx
+++ b/Sprint_5/FO.BD.GDC.SDC.005-001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sdc-docs\Spring_5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sdc-docs\Sprint_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4649,6 +4649,9 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Estimado</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln>
               <a:solidFill>
@@ -4659,6 +4662,28 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Product Backlog - option 1'!$F$5:$F$11</c:f>
@@ -4728,9 +4753,34 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Proyectado</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Product Backlog - option 1'!$F$5:$F$11</c:f>
@@ -4785,7 +4835,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4806,11 +4856,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="7919392"/>
-        <c:axId val="7926448"/>
+        <c:axId val="300515624"/>
+        <c:axId val="300512488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7919392"/>
+        <c:axId val="300515624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4830,7 +4880,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7926448"/>
+        <c:crossAx val="300512488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4839,7 +4889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7926448"/>
+        <c:axId val="300512488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4873,7 +4923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="7919392"/>
+        <c:crossAx val="300515624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5184,11 +5234,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="7922136"/>
-        <c:axId val="7919784"/>
+        <c:axId val="300514448"/>
+        <c:axId val="347104848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7922136"/>
+        <c:axId val="300514448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5208,7 +5258,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7919784"/>
+        <c:crossAx val="347104848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5217,7 +5267,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7919784"/>
+        <c:axId val="347104848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5244,7 +5294,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -5261,7 +5310,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7922136"/>
+        <c:crossAx val="300514448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5572,11 +5621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="7925664"/>
-        <c:axId val="7921352"/>
+        <c:axId val="347100928"/>
+        <c:axId val="347100536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7925664"/>
+        <c:axId val="347100928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5596,7 +5645,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7921352"/>
+        <c:crossAx val="347100536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5605,7 +5654,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7921352"/>
+        <c:axId val="347100536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5648,7 +5697,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7925664"/>
+        <c:crossAx val="347100928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5839,8 +5888,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="7923704"/>
-        <c:axId val="7926840"/>
+        <c:axId val="347099360"/>
+        <c:axId val="347106416"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5907,11 +5956,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="7921744"/>
-        <c:axId val="7922528"/>
+        <c:axId val="347102496"/>
+        <c:axId val="347100144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7923704"/>
+        <c:axId val="347099360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5977,7 +6026,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7926840"/>
+        <c:crossAx val="347106416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5985,7 +6034,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7926840"/>
+        <c:axId val="347106416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6044,12 +6093,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7923704"/>
+        <c:crossAx val="347099360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="7921744"/>
+        <c:axId val="347102496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6059,7 +6108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="7922528"/>
+        <c:crossAx val="347100144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6067,7 +6116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7922528"/>
+        <c:axId val="347100144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6105,7 +6154,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7921744"/>
+        <c:crossAx val="347102496"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6350,8 +6399,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="346441056"/>
-        <c:axId val="346442624"/>
+        <c:axId val="347102888"/>
+        <c:axId val="347101712"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6433,11 +6482,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="346439488"/>
-        <c:axId val="346441448"/>
+        <c:axId val="347103672"/>
+        <c:axId val="347103280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="346441056"/>
+        <c:axId val="347102888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6511,7 +6560,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346442624"/>
+        <c:crossAx val="347101712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6519,7 +6568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346442624"/>
+        <c:axId val="347101712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6578,12 +6627,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346441056"/>
+        <c:crossAx val="347102888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="346441448"/>
+        <c:axId val="347103280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6621,12 +6670,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346439488"/>
+        <c:crossAx val="347103672"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="346439488"/>
+        <c:axId val="347103672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6636,7 +6685,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="346441448"/>
+        <c:crossAx val="347103280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7133,14 +7182,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -7533,8 +7582,8 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="86" workbookViewId="0">
-      <pane ySplit="19" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
+      <pane ySplit="19" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7904,9 +7953,9 @@
       <c r="F11" s="199">
         <v>6</v>
       </c>
-      <c r="G11" s="181" t="str">
+      <c r="G11" s="181">
         <f>IF(COUNTIF(H$20:H1001,F11),SUMIF(H$20:H1001,F11,F$20:F1001),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="H11" s="169">
         <f t="shared" si="0"/>
@@ -7914,7 +7963,7 @@
       </c>
       <c r="I11" s="169">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J11" s="223">
         <f t="shared" si="4"/>
@@ -8491,7 +8540,9 @@
         <f t="shared" si="5"/>
         <v>79</v>
       </c>
-      <c r="H34" s="166"/>
+      <c r="H34" s="166">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="189">
@@ -8516,7 +8567,9 @@
         <f t="shared" si="5"/>
         <v>84</v>
       </c>
-      <c r="H35" s="166"/>
+      <c r="H35" s="166">
+        <v>6</v>
+      </c>
       <c r="I35" s="204">
         <f>A11</f>
         <v>43455</v>

</xml_diff>